<commit_message>
Ajustes para importação dos arquivos de Times e Jogadores, retirada de métodos desnecessários nas interfaces
</commit_message>
<xml_diff>
--- a/FURB.Basquete.Framework.Web/wwwroot/Upload/times-2018.xlsx
+++ b/FURB.Basquete.Framework.Web/wwwroot/Upload/times-2018.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaacnborges\Google Drive\Aula\FURB\TCC\planilhas\times\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA45C4C4-A898-4205-9286-59AF0DCDEFDE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832388BA-8E0C-4D02-B826-B19501F8F226}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{1F66DCAC-3338-4648-AB3F-D9542B6507C0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{1F66DCAC-3338-4648-AB3F-D9542B6507C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Per100" sheetId="2" r:id="rId1"/>
     <sheet name="Opponent Per 100" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Team Per100'!$B$1:$D$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Team Per100'!$B$1:$AA$31</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -2746,29 +2746,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C847DF-512D-4CB6-99BA-EE00C0C3640E}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2781,80 +2782,80 @@
       <c r="C1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>506</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2867,80 +2868,80 @@
       <c r="C2" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4">
+        <v>82</v>
+      </c>
+      <c r="E2" s="4">
+        <v>19730</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F2" s="4">
-        <v>82</v>
-      </c>
-      <c r="G2" s="4">
-        <v>19730</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2953,80 +2954,80 @@
       <c r="C3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7">
+        <v>82</v>
+      </c>
+      <c r="E3" s="7">
+        <v>19755</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="AB3" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F3" s="7">
-        <v>82</v>
-      </c>
-      <c r="G3" s="7">
-        <v>19755</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB3" s="8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3039,80 +3040,80 @@
       <c r="C4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7">
+        <v>82</v>
+      </c>
+      <c r="E4" s="7">
+        <v>19955</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="AB4" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F4" s="7">
-        <v>82</v>
-      </c>
-      <c r="G4" s="7">
-        <v>19955</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3125,80 +3126,80 @@
       <c r="C5" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7">
+        <v>82</v>
+      </c>
+      <c r="E5" s="7">
+        <v>19830</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="AB5" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F5" s="7">
-        <v>82</v>
-      </c>
-      <c r="G5" s="7">
-        <v>19830</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="V5" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z5" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB5" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3211,80 +3212,80 @@
       <c r="C6" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7">
+        <v>82</v>
+      </c>
+      <c r="E6" s="7">
+        <v>19730</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="AB6" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F6" s="7">
-        <v>82</v>
-      </c>
-      <c r="G6" s="7">
-        <v>19730</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB6" s="8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3297,80 +3298,80 @@
       <c r="C7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7">
+        <v>82</v>
+      </c>
+      <c r="E7" s="7">
+        <v>19880</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="V7" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="AB7" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F7" s="7">
-        <v>82</v>
-      </c>
-      <c r="G7" s="7">
-        <v>19880</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="X7" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="Z7" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA7" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB7" s="8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3383,80 +3384,80 @@
       <c r="C8" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7">
+        <v>82</v>
+      </c>
+      <c r="E8" s="7">
+        <v>19780</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="AB8" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F8" s="7">
-        <v>82</v>
-      </c>
-      <c r="G8" s="7">
-        <v>19780</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="U8" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="V8" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="X8" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y8" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z8" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA8" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB8" s="8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3469,80 +3470,80 @@
       <c r="C9" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7">
+        <v>82</v>
+      </c>
+      <c r="E9" s="7">
+        <v>19805</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="AB9" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F9" s="7">
-        <v>82</v>
-      </c>
-      <c r="G9" s="7">
-        <v>19805</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="V9" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="X9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z9" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB9" s="8" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3555,80 +3556,80 @@
       <c r="C10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7">
+        <v>82</v>
+      </c>
+      <c r="E10" s="7">
+        <v>19705</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="W10" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="AB10" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F10" s="7">
-        <v>82</v>
-      </c>
-      <c r="G10" s="7">
-        <v>19705</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U10" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="V10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="W10" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="X10" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y10" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z10" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="AA10" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="AB10" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3641,80 +3642,80 @@
       <c r="C11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7">
+        <v>82</v>
+      </c>
+      <c r="E11" s="7">
+        <v>19780</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="AB11" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F11" s="7">
-        <v>82</v>
-      </c>
-      <c r="G11" s="7">
-        <v>19780</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="U11" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="V11" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="W11" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="X11" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y11" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z11" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA11" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="AB11" s="8" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3727,80 +3728,80 @@
       <c r="C12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7">
+        <v>82</v>
+      </c>
+      <c r="E12" s="7">
+        <v>19905</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="AB12" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F12" s="7">
-        <v>82</v>
-      </c>
-      <c r="G12" s="7">
-        <v>19905</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="T12" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="W12" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="X12" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="Z12" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA12" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="AB12" s="8" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3813,80 +3814,80 @@
       <c r="C13" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7">
+        <v>82</v>
+      </c>
+      <c r="E13" s="7">
+        <v>19830</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="AB13" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F13" s="7">
-        <v>82</v>
-      </c>
-      <c r="G13" s="7">
-        <v>19830</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="X13" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="Y13" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="Z13" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="AA13" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="AB13" s="8" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3899,80 +3900,80 @@
       <c r="C14" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="7">
+        <v>82</v>
+      </c>
+      <c r="E14" s="7">
+        <v>19855</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="V14" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="AA14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="AB14" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F14" s="7">
-        <v>82</v>
-      </c>
-      <c r="G14" s="7">
-        <v>19855</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U14" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="V14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="X14" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="Y14" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z14" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="AA14" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="AB14" s="8" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3985,80 +3986,80 @@
       <c r="C15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7">
+        <v>82</v>
+      </c>
+      <c r="E15" s="7">
+        <v>19855</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="AA15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="AB15" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F15" s="7">
-        <v>82</v>
-      </c>
-      <c r="G15" s="7">
-        <v>19855</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="V15" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="W15" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="X15" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y15" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="Z15" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="AA15" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB15" s="8" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4071,80 +4072,80 @@
       <c r="C16" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7">
+        <v>82</v>
+      </c>
+      <c r="E16" s="7">
+        <v>19830</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="AB16" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F16" s="7">
-        <v>82</v>
-      </c>
-      <c r="G16" s="7">
-        <v>19830</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q16" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="X16" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="Y16" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="Z16" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="AA16" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB16" s="8" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4157,80 +4158,80 @@
       <c r="C17" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="7">
+        <v>82</v>
+      </c>
+      <c r="E17" s="7">
+        <v>19755</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="AA17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="AB17" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F17" s="7">
-        <v>82</v>
-      </c>
-      <c r="G17" s="7">
-        <v>19755</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="U17" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="V17" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="W17" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="X17" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y17" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="Z17" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="AA17" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="AB17" s="8" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4243,80 +4244,80 @@
       <c r="C18" s="16" t="s">
         <v>357</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="7">
+        <v>82</v>
+      </c>
+      <c r="E18" s="7">
+        <v>19755</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="W18" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y18" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="AB18" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F18" s="7">
-        <v>82</v>
-      </c>
-      <c r="G18" s="7">
-        <v>19755</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="U18" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="V18" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="W18" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="X18" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="Y18" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="Z18" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="AA18" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="AB18" s="8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4329,80 +4330,80 @@
       <c r="C19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="7">
+        <v>82</v>
+      </c>
+      <c r="E19" s="7">
+        <v>19830</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="AA19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="AB19" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F19" s="7">
-        <v>82</v>
-      </c>
-      <c r="G19" s="7">
-        <v>19830</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="U19" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="V19" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="X19" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="Z19" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="AA19" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="AB19" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4415,80 +4416,80 @@
       <c r="C20" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7">
+        <v>82</v>
+      </c>
+      <c r="E20" s="7">
+        <v>19755</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="W20" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="X20" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="AA20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="AB20" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F20" s="7">
-        <v>82</v>
-      </c>
-      <c r="G20" s="7">
-        <v>19755</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="S20" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="X20" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="Y20" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="Z20" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA20" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB20" s="8" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4501,80 +4502,80 @@
       <c r="C21" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="7">
+        <v>82</v>
+      </c>
+      <c r="E21" s="7">
+        <v>19805</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="AA21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="AB21" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F21" s="7">
-        <v>82</v>
-      </c>
-      <c r="G21" s="7">
-        <v>19805</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="S21" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="T21" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="U21" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="V21" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="W21" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="X21" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="Y21" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="Z21" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="AA21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB21" s="8" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4587,80 +4588,80 @@
       <c r="C22" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7">
+        <v>82</v>
+      </c>
+      <c r="E22" s="7">
+        <v>19705</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="W22" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z22" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="AA22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="AB22" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F22" s="7">
-        <v>82</v>
-      </c>
-      <c r="G22" s="7">
-        <v>19705</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="V22" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="X22" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y22" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="Z22" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="AA22" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="AB22" s="8" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4673,80 +4674,80 @@
       <c r="C23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7">
+        <v>82</v>
+      </c>
+      <c r="E23" s="7">
+        <v>19805</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="Z23" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="AB23" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F23" s="7">
-        <v>82</v>
-      </c>
-      <c r="G23" s="7">
-        <v>19805</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="S23" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="U23" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="V23" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="W23" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="X23" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y23" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="Z23" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="AA23" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="AB23" s="8" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4759,80 +4760,80 @@
       <c r="C24" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7">
+        <v>82</v>
+      </c>
+      <c r="E24" s="7">
+        <v>19930</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="V24" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z24" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="AB24" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F24" s="7">
-        <v>82</v>
-      </c>
-      <c r="G24" s="7">
-        <v>19930</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="S24" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="T24" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="U24" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="V24" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="W24" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="X24" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y24" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="Z24" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="AA24" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="AB24" s="8" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4845,80 +4846,80 @@
       <c r="C25" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="7">
+        <v>82</v>
+      </c>
+      <c r="E25" s="7">
+        <v>19730</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z25" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="AA25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="AB25" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F25" s="7">
-        <v>82</v>
-      </c>
-      <c r="G25" s="7">
-        <v>19730</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="N25" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="R25" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="S25" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="T25" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="U25" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="V25" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="X25" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y25" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="Z25" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="AA25" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB25" s="8" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4931,80 +4932,80 @@
       <c r="C26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="7">
+        <v>82</v>
+      </c>
+      <c r="E26" s="7">
+        <v>19705</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="V26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z26" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="AA26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="AB26" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F26" s="7">
-        <v>82</v>
-      </c>
-      <c r="G26" s="7">
-        <v>19705</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M26" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="N26" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="O26" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="U26" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="V26" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="W26" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="X26" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y26" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="Z26" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA26" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB26" s="8" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5017,80 +5018,80 @@
       <c r="C27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="7">
+        <v>82</v>
+      </c>
+      <c r="E27" s="7">
+        <v>19855</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="Z27" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="AA27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="AB27" s="17" t="s">
         <v>508</v>
-      </c>
-      <c r="F27" s="7">
-        <v>82</v>
-      </c>
-      <c r="G27" s="7">
-        <v>19855</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>460</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="M27" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="P27" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="S27" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="U27" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="V27" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="W27" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="X27" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y27" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="Z27" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA27" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB27" s="8" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5103,80 +5104,80 @@
       <c r="C28" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="7">
+        <v>82</v>
+      </c>
+      <c r="E28" s="7">
+        <v>19730</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="U28" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="AA28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="AB28" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F28" s="7">
-        <v>82</v>
-      </c>
-      <c r="G28" s="7">
-        <v>19730</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="O28" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="P28" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="R28" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="S28" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="T28" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="U28" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="V28" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="W28" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="X28" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y28" s="7" t="s">
-        <v>480</v>
-      </c>
-      <c r="Z28" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="AA28" s="7" t="s">
-        <v>481</v>
-      </c>
-      <c r="AB28" s="8" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5189,80 +5190,80 @@
       <c r="C29" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="7">
+        <v>82</v>
+      </c>
+      <c r="E29" s="7">
+        <v>19805</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z29" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="AA29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="AB29" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F29" s="7">
-        <v>82</v>
-      </c>
-      <c r="G29" s="7">
-        <v>19805</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="R29" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>487</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="U29" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="V29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="W29" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="X29" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="Y29" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z29" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA29" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB29" s="8" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5275,80 +5276,80 @@
       <c r="C30" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="7">
+        <v>82</v>
+      </c>
+      <c r="E30" s="7">
+        <v>19705</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="S30" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="U30" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="W30" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="X30" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="Y30" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="Z30" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="AB30" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F30" s="7">
-        <v>82</v>
-      </c>
-      <c r="G30" s="7">
-        <v>19705</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="P30" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="R30" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="U30" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="W30" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="X30" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y30" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z30" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="AA30" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="AB30" s="8" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5361,80 +5362,80 @@
       <c r="C31" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="10">
+        <v>82</v>
+      </c>
+      <c r="E31" s="10">
+        <v>19755</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="P31" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="T31" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="V31" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="W31" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="X31" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y31" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z31" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="AA31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="AB31" s="16" t="s">
         <v>507</v>
-      </c>
-      <c r="F31" s="10">
-        <v>82</v>
-      </c>
-      <c r="G31" s="10">
-        <v>19755</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="L31" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="N31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="O31" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="P31" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q31" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="R31" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="S31" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="T31" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="U31" s="10" t="s">
-        <v>502</v>
-      </c>
-      <c r="V31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="W31" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="X31" s="10" t="s">
-        <v>503</v>
-      </c>
-      <c r="Y31" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z31" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="AA31" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="AB31" s="11" t="s">
-        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -5447,7 +5448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27165C7-C463-4671-A9D6-12B58A6D0E1C}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>